<commit_message>
Adjusted colors and labels to fit other group member's work
</commit_message>
<xml_diff>
--- a/Result Tables/results.diff.2019.xlsx
+++ b/Result Tables/results.diff.2019.xlsx
@@ -17,10 +17,10 @@
     <t xml:space="preserve">parameter</t>
   </si>
   <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
+    <t xml:space="preserve">Kiefer (n. entb.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiefer (entb.)</t>
   </si>
   <si>
     <t xml:space="preserve">Buche</t>
@@ -41,10 +41,10 @@
     <t xml:space="preserve">Signif</t>
   </si>
   <si>
-    <t xml:space="preserve">2018.letter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013.letter</t>
+    <t xml:space="preserve">Kiefer (n. entb.).letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiefer (entb.).letter</t>
   </si>
   <si>
     <t xml:space="preserve">Buche.letter</t>

</xml_diff>